<commit_message>
Fixed search function with failed search display
</commit_message>
<xml_diff>
--- a/avg_dump/BatteryProduct.xlsx
+++ b/avg_dump/BatteryProduct.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kobe\Desktop\My Family FIles\kobe files\programming files\LaravelApps\Mass-V-Group-Inc\avg_dump\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D845580-B9D7-41C8-86AC-26073A618547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A69551F-AA0A-4060-9A51-3A60612BB060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7110" yWindow="2100" windowWidth="18390" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="129">
   <si>
     <r>
       <rPr>
@@ -932,15 +932,6 @@
     <t>WARRANTY</t>
   </si>
   <si>
-    <t>assets/New Mega Force LM.png</t>
-  </si>
-  <si>
-    <t>assets/New Megaforce MF.png</t>
-  </si>
-  <si>
-    <t>assets/Mega Force Plus.png</t>
-  </si>
-  <si>
     <t>assets/Primera.png</t>
   </si>
   <si>
@@ -969,6 +960,66 @@
   </si>
   <si>
     <t>SuperKing</t>
+  </si>
+  <si>
+    <t>DIN44</t>
+  </si>
+  <si>
+    <t>DIN55</t>
+  </si>
+  <si>
+    <t>DIN55R</t>
+  </si>
+  <si>
+    <t>DIN74</t>
+  </si>
+  <si>
+    <t>NX110-5L / NX110-5</t>
+  </si>
+  <si>
+    <t>NX120-7 / NX120-7L</t>
+  </si>
+  <si>
+    <t>NS40Z / NS40L</t>
+  </si>
+  <si>
+    <t>NS60L / NS60R</t>
+  </si>
+  <si>
+    <t>NT80L / NT80R</t>
+  </si>
+  <si>
+    <t>40B20L / 40B20R</t>
+  </si>
+  <si>
+    <t>46B24L / 46B24R</t>
+  </si>
+  <si>
+    <t>55B24L / 55B24R</t>
+  </si>
+  <si>
+    <t>65D26 / 65D26L</t>
+  </si>
+  <si>
+    <t>80D26 / 80D26L</t>
+  </si>
+  <si>
+    <t>95D31 / 95D31L</t>
+  </si>
+  <si>
+    <t>105D31 / 105D31L</t>
+  </si>
+  <si>
+    <t>G65 / 65-750</t>
+  </si>
+  <si>
+    <t>assets/MegaForce_LM.png</t>
+  </si>
+  <si>
+    <t>assets/Megaforce_MF.png</t>
+  </si>
+  <si>
+    <t>assets/MegaForce_PLUS.png</t>
   </si>
 </sst>
 </file>
@@ -986,15 +1037,18 @@
       <i/>
       <sz val="8.5"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8.5"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8.5"/>
@@ -1845,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA45D5D-432F-4145-822B-5103900648A4}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1860,7 +1914,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
         <v>96</v>
@@ -1872,12 +1926,12 @@
         <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>89</v>
@@ -1889,12 +1943,12 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -1906,12 +1960,12 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
@@ -1923,12 +1977,12 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>88</v>
@@ -1940,12 +1994,12 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>19</v>
@@ -1957,12 +2011,12 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
@@ -1974,12 +2028,12 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -1991,63 +2045,63 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>73</v>
@@ -2059,83 +2113,83 @@
         <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="C17" s="3">
         <v>54434</v>
@@ -2144,15 +2198,15 @@
         <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
+        <v>127</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="C18" s="3">
         <v>55559</v>
@@ -2161,15 +2215,15 @@
         <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>127</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="C19" s="3">
         <v>55565</v>
@@ -2178,15 +2232,15 @@
         <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>127</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="C20" s="3">
         <v>57412</v>
@@ -2195,12 +2249,12 @@
         <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>30</v>
@@ -2212,12 +2266,12 @@
         <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>31</v>
@@ -2229,29 +2283,29 @@
         <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>33</v>
+      <c r="C23" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>34</v>
@@ -2263,12 +2317,12 @@
         <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>90</v>
@@ -2280,12 +2334,12 @@
         <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>38</v>
@@ -2297,12 +2351,12 @@
         <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>91</v>
@@ -2314,12 +2368,12 @@
         <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>92</v>
@@ -2331,12 +2385,12 @@
         <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>42</v>
@@ -2348,12 +2402,12 @@
         <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>12</v>
@@ -2365,12 +2419,12 @@
         <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>46</v>
@@ -2382,12 +2436,12 @@
         <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>48</v>
@@ -2399,12 +2453,12 @@
         <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>50</v>
@@ -2416,12 +2470,12 @@
         <v>44</v>
       </c>
       <c r="E33" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>52</v>
@@ -2433,12 +2487,12 @@
         <v>44</v>
       </c>
       <c r="E34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>54</v>
@@ -2447,15 +2501,15 @@
         <v>55</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E35" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>56</v>
@@ -2467,12 +2521,12 @@
         <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>58</v>
@@ -2484,12 +2538,12 @@
         <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>42</v>
@@ -2501,12 +2555,12 @@
         <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>12</v>
@@ -2518,12 +2572,12 @@
         <v>62</v>
       </c>
       <c r="E39" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>48</v>
@@ -2535,12 +2589,12 @@
         <v>62</v>
       </c>
       <c r="E40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>50</v>
@@ -2552,12 +2606,12 @@
         <v>62</v>
       </c>
       <c r="E41" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>52</v>
@@ -2569,12 +2623,12 @@
         <v>62</v>
       </c>
       <c r="E42" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>54</v>
@@ -2586,12 +2640,12 @@
         <v>62</v>
       </c>
       <c r="E43" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>56</v>
@@ -2603,12 +2657,12 @@
         <v>62</v>
       </c>
       <c r="E44" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>58</v>
@@ -2620,7 +2674,7 @@
         <v>62</v>
       </c>
       <c r="E45" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2633,7 +2687,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16:J23"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3525,7 +3579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="J14" sqref="J14:J29"/>
     </sheetView>
   </sheetViews>

</xml_diff>